<commit_message>
update datasheets and docu
</commit_message>
<xml_diff>
--- a/development/Requirements.xlsx
+++ b/development/Requirements.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2_Momo\30_RC_Planes\40_DIY ELRS and FC\13_FC STM32H7xx Gliwa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2_Momo\30_RC_Planes\40_DIY ELRS and FC\13_MoGliFC_git\MoGliFC\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF73FF1-960F-4078-B041-E842A02F98CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A62E16-7649-4A6E-9880-22AB9EC0F8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="1" r:id="rId1"/>
     <sheet name="H743 target definition" sheetId="2" r:id="rId2"/>
+    <sheet name="Power calc" sheetId="3" r:id="rId3"/>
+    <sheet name="price" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="137">
   <si>
     <t>domain</t>
   </si>
@@ -339,12 +341,114 @@
   </si>
   <si>
     <t>1x</t>
+  </si>
+  <si>
+    <t>Calculated max. Power per component/rail</t>
+  </si>
+  <si>
+    <t>STM32H7</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>Mag</t>
+  </si>
+  <si>
+    <t>3V3 FC:</t>
+  </si>
+  <si>
+    <t>external</t>
+  </si>
+  <si>
+    <t>ELRS:</t>
+  </si>
+  <si>
+    <t>ESP32 pico D4</t>
+  </si>
+  <si>
+    <t>SX1280 1</t>
+  </si>
+  <si>
+    <t>AT2401C 1</t>
+  </si>
+  <si>
+    <t>SX1280 2</t>
+  </si>
+  <si>
+    <t>AT2401C 2</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>Architecture:</t>
+  </si>
+  <si>
+    <t>Ubat</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>3V3</t>
+  </si>
+  <si>
+    <t>U [V]</t>
+  </si>
+  <si>
+    <t>I[A]</t>
+  </si>
+  <si>
+    <t>P_loss[W]</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>LDO loss:</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>flash</t>
+  </si>
+  <si>
+    <t>BEC 5V FC</t>
+  </si>
+  <si>
+    <t>BEC 5V Vx</t>
+  </si>
+  <si>
+    <t>BEC 10V</t>
+  </si>
+  <si>
+    <t>LDOs</t>
+  </si>
+  <si>
+    <t>Baro DPS310</t>
+  </si>
+  <si>
+    <t>BMI270</t>
+  </si>
+  <si>
+    <t>AT7456 OSD</t>
+  </si>
+  <si>
+    <t>SUMME</t>
+  </si>
+  <si>
+    <t>zeugs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00\ \A"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -454,9 +558,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -739,7 +844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
@@ -897,7 +1002,7 @@
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="5" t="s">
         <v>101</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -1572,4 +1677,350 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EB0395-419A-4274-917D-83467D3B0DCC}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <f>SUM(B5:J5)</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="C20" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="14">
+        <f>(C23-C25) * D25</f>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25">
+        <v>3.3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908C4812-EFC0-413C-8EA6-EC194AA8244F}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B1:B16)</f>
+        <v>30.000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>